<commit_message>
missing edits from mohamed osama
</commit_message>
<xml_diff>
--- a/New Microsoft Excel Worksheet.xlsx
+++ b/New Microsoft Excel Worksheet.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Clients\New folder (3)\New folder (3)\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37C23947-9547-421F-817B-67850D79BBF1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-240" yWindow="150" windowWidth="21855" windowHeight="12495" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-240" yWindow="150" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="MH" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -884,12 +878,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -908,7 +902,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -931,11 +925,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -943,11 +948,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" readingOrder="2"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1046,7 +1061,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1081,7 +1096,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1258,23 +1273,27 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
-      <selection activeCell="E195" sqref="E195"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1330,7 +1349,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1382,7 +1401,7 @@
       </c>
       <c r="R2" s="1"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1434,7 +1453,7 @@
       </c>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1486,7 +1505,7 @@
       </c>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1511,17 +1530,17 @@
       <c r="H5" s="1">
         <v>0</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="3">
+        <v>0</v>
+      </c>
+      <c r="J5" s="1">
+        <v>0</v>
+      </c>
+      <c r="K5" s="1">
+        <v>0</v>
+      </c>
+      <c r="L5" s="1">
         <v>0.5</v>
-      </c>
-      <c r="J5" s="1">
-        <v>0</v>
-      </c>
-      <c r="K5" s="1">
-        <v>0</v>
-      </c>
-      <c r="L5" s="1">
-        <v>0</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>21</v>
@@ -1538,7 +1557,7 @@
       </c>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1590,7 +1609,7 @@
       </c>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1642,7 +1661,7 @@
       </c>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1694,7 +1713,7 @@
       </c>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1746,7 +1765,7 @@
       </c>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1798,7 +1817,7 @@
       </c>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1850,7 +1869,7 @@
       </c>
       <c r="R11" s="1"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1902,7 +1921,7 @@
       </c>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1954,7 +1973,7 @@
       </c>
       <c r="R13" s="1"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2006,7 +2025,7 @@
       </c>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2058,7 +2077,7 @@
       </c>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2110,7 +2129,7 @@
       </c>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2162,7 +2181,7 @@
       </c>
       <c r="R17" s="1"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2214,7 +2233,7 @@
       </c>
       <c r="R18" s="1"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2266,7 +2285,7 @@
       </c>
       <c r="R19" s="1"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2318,7 +2337,7 @@
       </c>
       <c r="R20" s="1"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2370,7 +2389,7 @@
       </c>
       <c r="R21" s="1"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2422,7 +2441,7 @@
       </c>
       <c r="R22" s="1"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2474,7 +2493,7 @@
       </c>
       <c r="R23" s="1"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2526,7 +2545,7 @@
       </c>
       <c r="R24" s="1"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2578,7 +2597,7 @@
       </c>
       <c r="R25" s="1"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2630,7 +2649,7 @@
       </c>
       <c r="R26" s="1"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2682,7 +2701,7 @@
       </c>
       <c r="R27" s="1"/>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2734,7 +2753,7 @@
       </c>
       <c r="R28" s="1"/>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2786,7 +2805,7 @@
       </c>
       <c r="R29" s="1"/>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2838,7 +2857,7 @@
       </c>
       <c r="R30" s="1"/>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2890,7 +2909,7 @@
       </c>
       <c r="R31" s="1"/>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2942,7 +2961,7 @@
       </c>
       <c r="R32" s="1"/>
     </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2994,7 +3013,7 @@
       </c>
       <c r="R33" s="1"/>
     </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -3046,7 +3065,7 @@
       </c>
       <c r="R34" s="1"/>
     </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -3098,7 +3117,7 @@
       </c>
       <c r="R35" s="1"/>
     </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>35</v>
       </c>
@@ -3150,7 +3169,7 @@
       </c>
       <c r="R36" s="1"/>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -3202,7 +3221,7 @@
       </c>
       <c r="R37" s="1"/>
     </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -3254,7 +3273,7 @@
       </c>
       <c r="R38" s="1"/>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -3306,7 +3325,7 @@
       </c>
       <c r="R39" s="1"/>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -3358,7 +3377,7 @@
       </c>
       <c r="R40" s="1"/>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -3410,7 +3429,7 @@
       </c>
       <c r="R41" s="1"/>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -3462,7 +3481,7 @@
       </c>
       <c r="R42" s="1"/>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -3514,7 +3533,7 @@
       </c>
       <c r="R43" s="1"/>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -3566,7 +3585,7 @@
       </c>
       <c r="R44" s="1"/>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -3618,7 +3637,7 @@
       </c>
       <c r="R45" s="1"/>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -3670,7 +3689,7 @@
       </c>
       <c r="R46" s="1"/>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -3722,7 +3741,7 @@
       </c>
       <c r="R47" s="1"/>
     </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -3774,7 +3793,7 @@
       </c>
       <c r="R48" s="1"/>
     </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -3828,7 +3847,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -3880,7 +3899,7 @@
       </c>
       <c r="R50" s="1"/>
     </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -3934,7 +3953,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -3988,7 +4007,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -4040,7 +4059,7 @@
       </c>
       <c r="R53" s="1"/>
     </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -4092,7 +4111,7 @@
       </c>
       <c r="R54" s="1"/>
     </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -4144,7 +4163,7 @@
       </c>
       <c r="R55" s="1"/>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -4196,7 +4215,7 @@
       </c>
       <c r="R56" s="1"/>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -4250,7 +4269,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -4304,7 +4323,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -4356,7 +4375,7 @@
       </c>
       <c r="R59" s="1"/>
     </row>
-    <row r="60" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -4410,7 +4429,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="61" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -4466,7 +4485,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="62" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -4520,7 +4539,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -4572,7 +4591,7 @@
       </c>
       <c r="R63" s="1"/>
     </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -4626,7 +4645,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -4678,7 +4697,7 @@
       </c>
       <c r="R65" s="1"/>
     </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -4732,7 +4751,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -4784,7 +4803,7 @@
       </c>
       <c r="R67" s="1"/>
     </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -4836,7 +4855,7 @@
       </c>
       <c r="R68" s="1"/>
     </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -4890,7 +4909,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -4942,7 +4961,7 @@
       </c>
       <c r="R70" s="1"/>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -4996,7 +5015,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -5050,7 +5069,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -5104,7 +5123,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -5158,7 +5177,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -5210,7 +5229,7 @@
       </c>
       <c r="R75" s="1"/>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -5264,7 +5283,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -5318,7 +5337,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -5372,7 +5391,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -5426,7 +5445,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -5478,7 +5497,7 @@
       </c>
       <c r="R80" s="1"/>
     </row>
-    <row r="81" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -5532,7 +5551,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="82" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -5586,7 +5605,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="83" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -5638,7 +5657,7 @@
       </c>
       <c r="R83" s="1"/>
     </row>
-    <row r="84" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -5692,7 +5711,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="85" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -5746,7 +5765,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="86" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -5800,7 +5819,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="87" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -5852,7 +5871,7 @@
       </c>
       <c r="R87" s="1"/>
     </row>
-    <row r="88" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -5906,7 +5925,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="89" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -5958,7 +5977,7 @@
       </c>
       <c r="R89" s="1"/>
     </row>
-    <row r="90" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -6010,7 +6029,7 @@
       </c>
       <c r="R90" s="1"/>
     </row>
-    <row r="91" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -6062,7 +6081,7 @@
       </c>
       <c r="R91" s="1"/>
     </row>
-    <row r="92" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -6116,7 +6135,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="93" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -6168,7 +6187,7 @@
       </c>
       <c r="R93" s="1"/>
     </row>
-    <row r="94" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -6222,7 +6241,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="95" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -6274,7 +6293,7 @@
       </c>
       <c r="R95" s="1"/>
     </row>
-    <row r="96" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -6328,7 +6347,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="97" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -6382,7 +6401,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="98" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -6436,7 +6455,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="99" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -6488,7 +6507,7 @@
       </c>
       <c r="R99" s="1"/>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -6540,7 +6559,7 @@
       </c>
       <c r="R100" s="1"/>
     </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -6594,7 +6613,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -6648,7 +6667,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="103" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -6700,7 +6719,7 @@
       </c>
       <c r="R103" s="1"/>
     </row>
-    <row r="104" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -6752,7 +6771,7 @@
       </c>
       <c r="R104" s="1"/>
     </row>
-    <row r="105" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -6806,7 +6825,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="106" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -6858,7 +6877,7 @@
       </c>
       <c r="R106" s="1"/>
     </row>
-    <row r="107" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -6910,7 +6929,7 @@
       </c>
       <c r="R107" s="1"/>
     </row>
-    <row r="108" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>107</v>
       </c>
@@ -6962,7 +6981,7 @@
       </c>
       <c r="R108" s="1"/>
     </row>
-    <row r="109" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>108</v>
       </c>
@@ -7016,7 +7035,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="110" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>109</v>
       </c>
@@ -7068,7 +7087,7 @@
       </c>
       <c r="R110" s="1"/>
     </row>
-    <row r="111" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>110</v>
       </c>
@@ -7122,7 +7141,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="112" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>111</v>
       </c>
@@ -7174,7 +7193,7 @@
       </c>
       <c r="R112" s="1"/>
     </row>
-    <row r="113" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>112</v>
       </c>
@@ -7226,7 +7245,7 @@
       </c>
       <c r="R113" s="1"/>
     </row>
-    <row r="114" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>113</v>
       </c>
@@ -7278,7 +7297,7 @@
       </c>
       <c r="R114" s="1"/>
     </row>
-    <row r="115" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>114</v>
       </c>
@@ -7332,7 +7351,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="116" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>115</v>
       </c>
@@ -7384,7 +7403,7 @@
       </c>
       <c r="R116" s="1"/>
     </row>
-    <row r="117" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>116</v>
       </c>
@@ -7438,7 +7457,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="118" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>117</v>
       </c>
@@ -7490,7 +7509,7 @@
       </c>
       <c r="R118" s="1"/>
     </row>
-    <row r="119" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>118</v>
       </c>
@@ -7544,7 +7563,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="120" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>119</v>
       </c>
@@ -7598,7 +7617,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="121" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>120</v>
       </c>
@@ -7650,7 +7669,7 @@
       </c>
       <c r="R121" s="1"/>
     </row>
-    <row r="122" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>121</v>
       </c>
@@ -7702,7 +7721,7 @@
       </c>
       <c r="R122" s="1"/>
     </row>
-    <row r="123" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>122</v>
       </c>
@@ -7754,7 +7773,7 @@
       </c>
       <c r="R123" s="1"/>
     </row>
-    <row r="124" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>123</v>
       </c>
@@ -7806,7 +7825,7 @@
       </c>
       <c r="R124" s="1"/>
     </row>
-    <row r="125" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>124</v>
       </c>
@@ -7860,7 +7879,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="126" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>125</v>
       </c>
@@ -7914,7 +7933,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="127" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>126</v>
       </c>
@@ -7966,7 +7985,7 @@
       </c>
       <c r="R127" s="1"/>
     </row>
-    <row r="128" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>127</v>
       </c>
@@ -8020,7 +8039,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="129" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>128</v>
       </c>
@@ -8072,7 +8091,7 @@
       </c>
       <c r="R129" s="1"/>
     </row>
-    <row r="130" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>129</v>
       </c>
@@ -8126,7 +8145,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="131" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>130</v>
       </c>
@@ -8178,7 +8197,7 @@
       </c>
       <c r="R131" s="1"/>
     </row>
-    <row r="132" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>131</v>
       </c>
@@ -8230,7 +8249,7 @@
       </c>
       <c r="R132" s="1"/>
     </row>
-    <row r="133" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>132</v>
       </c>
@@ -8282,7 +8301,7 @@
       </c>
       <c r="R133" s="1"/>
     </row>
-    <row r="134" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>133</v>
       </c>
@@ -8334,7 +8353,7 @@
       </c>
       <c r="R134" s="1"/>
     </row>
-    <row r="135" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>134</v>
       </c>
@@ -8386,7 +8405,7 @@
       </c>
       <c r="R135" s="1"/>
     </row>
-    <row r="136" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>135</v>
       </c>
@@ -8438,7 +8457,7 @@
       </c>
       <c r="R136" s="1"/>
     </row>
-    <row r="137" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>136</v>
       </c>
@@ -8490,7 +8509,7 @@
       </c>
       <c r="R137" s="1"/>
     </row>
-    <row r="138" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>137</v>
       </c>
@@ -8542,7 +8561,7 @@
       </c>
       <c r="R138" s="1"/>
     </row>
-    <row r="139" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>138</v>
       </c>
@@ -8594,7 +8613,7 @@
       </c>
       <c r="R139" s="1"/>
     </row>
-    <row r="140" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>139</v>
       </c>
@@ -8646,7 +8665,7 @@
       </c>
       <c r="R140" s="1"/>
     </row>
-    <row r="141" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>140</v>
       </c>
@@ -8698,7 +8717,7 @@
       </c>
       <c r="R141" s="1"/>
     </row>
-    <row r="142" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>141</v>
       </c>
@@ -8750,7 +8769,7 @@
       </c>
       <c r="R142" s="1"/>
     </row>
-    <row r="143" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>142</v>
       </c>
@@ -8802,7 +8821,7 @@
       </c>
       <c r="R143" s="1"/>
     </row>
-    <row r="144" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>143</v>
       </c>
@@ -8854,7 +8873,7 @@
       </c>
       <c r="R144" s="1"/>
     </row>
-    <row r="145" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>144</v>
       </c>
@@ -8906,7 +8925,7 @@
       </c>
       <c r="R145" s="1"/>
     </row>
-    <row r="146" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>145</v>
       </c>
@@ -8958,7 +8977,7 @@
       </c>
       <c r="R146" s="1"/>
     </row>
-    <row r="147" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>146</v>
       </c>
@@ -9010,7 +9029,7 @@
       </c>
       <c r="R147" s="1"/>
     </row>
-    <row r="148" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>147</v>
       </c>
@@ -9062,7 +9081,7 @@
       </c>
       <c r="R148" s="1"/>
     </row>
-    <row r="149" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>148</v>
       </c>
@@ -9114,7 +9133,7 @@
       </c>
       <c r="R149" s="1"/>
     </row>
-    <row r="150" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>149</v>
       </c>
@@ -9166,7 +9185,7 @@
       </c>
       <c r="R150" s="1"/>
     </row>
-    <row r="151" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>150</v>
       </c>
@@ -9218,7 +9237,7 @@
       </c>
       <c r="R151" s="1"/>
     </row>
-    <row r="152" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>151</v>
       </c>
@@ -9270,7 +9289,7 @@
       </c>
       <c r="R152" s="1"/>
     </row>
-    <row r="153" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>152</v>
       </c>
@@ -9322,7 +9341,7 @@
       </c>
       <c r="R153" s="1"/>
     </row>
-    <row r="154" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>153</v>
       </c>
@@ -9374,7 +9393,7 @@
       </c>
       <c r="R154" s="1"/>
     </row>
-    <row r="155" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>154</v>
       </c>
@@ -9426,7 +9445,7 @@
       </c>
       <c r="R155" s="1"/>
     </row>
-    <row r="156" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>155</v>
       </c>
@@ -9478,7 +9497,7 @@
       </c>
       <c r="R156" s="1"/>
     </row>
-    <row r="157" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>156</v>
       </c>
@@ -9530,7 +9549,7 @@
       </c>
       <c r="R157" s="1"/>
     </row>
-    <row r="158" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>157</v>
       </c>
@@ -9582,7 +9601,7 @@
       </c>
       <c r="R158" s="1"/>
     </row>
-    <row r="159" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>158</v>
       </c>
@@ -9634,7 +9653,7 @@
       </c>
       <c r="R159" s="1"/>
     </row>
-    <row r="160" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>159</v>
       </c>
@@ -9686,7 +9705,7 @@
       </c>
       <c r="R160" s="1"/>
     </row>
-    <row r="161" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>160</v>
       </c>
@@ -9738,7 +9757,7 @@
       </c>
       <c r="R161" s="1"/>
     </row>
-    <row r="162" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>161</v>
       </c>
@@ -9790,7 +9809,7 @@
       </c>
       <c r="R162" s="1"/>
     </row>
-    <row r="163" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>162</v>
       </c>
@@ -9842,7 +9861,7 @@
       </c>
       <c r="R163" s="1"/>
     </row>
-    <row r="164" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>163</v>
       </c>
@@ -9894,7 +9913,7 @@
       </c>
       <c r="R164" s="1"/>
     </row>
-    <row r="165" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>164</v>
       </c>
@@ -9946,7 +9965,7 @@
       </c>
       <c r="R165" s="1"/>
     </row>
-    <row r="166" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>165</v>
       </c>
@@ -9998,7 +10017,7 @@
       </c>
       <c r="R166" s="1"/>
     </row>
-    <row r="167" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>166</v>
       </c>
@@ -10050,7 +10069,7 @@
       </c>
       <c r="R167" s="1"/>
     </row>
-    <row r="168" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>167</v>
       </c>
@@ -10102,7 +10121,7 @@
       </c>
       <c r="R168" s="1"/>
     </row>
-    <row r="169" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>168</v>
       </c>
@@ -10154,7 +10173,7 @@
       </c>
       <c r="R169" s="1"/>
     </row>
-    <row r="170" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>169</v>
       </c>
@@ -10206,7 +10225,7 @@
       </c>
       <c r="R170" s="1"/>
     </row>
-    <row r="171" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>170</v>
       </c>
@@ -10258,7 +10277,7 @@
       </c>
       <c r="R171" s="1"/>
     </row>
-    <row r="172" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>171</v>
       </c>
@@ -10310,7 +10329,7 @@
       </c>
       <c r="R172" s="1"/>
     </row>
-    <row r="173" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>172</v>
       </c>
@@ -10362,7 +10381,7 @@
       </c>
       <c r="R173" s="1"/>
     </row>
-    <row r="174" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>173</v>
       </c>
@@ -10414,7 +10433,7 @@
       </c>
       <c r="R174" s="1"/>
     </row>
-    <row r="175" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>174</v>
       </c>
@@ -10466,7 +10485,7 @@
       </c>
       <c r="R175" s="1"/>
     </row>
-    <row r="176" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>175</v>
       </c>
@@ -10518,7 +10537,7 @@
       </c>
       <c r="R176" s="1"/>
     </row>
-    <row r="177" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>176</v>
       </c>
@@ -10570,7 +10589,7 @@
       </c>
       <c r="R177" s="1"/>
     </row>
-    <row r="178" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>177</v>
       </c>
@@ -10622,7 +10641,7 @@
       </c>
       <c r="R178" s="1"/>
     </row>
-    <row r="179" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>178</v>
       </c>
@@ -10674,7 +10693,7 @@
       </c>
       <c r="R179" s="1"/>
     </row>
-    <row r="180" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>179</v>
       </c>
@@ -10726,7 +10745,7 @@
       </c>
       <c r="R180" s="1"/>
     </row>
-    <row r="181" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>180</v>
       </c>
@@ -10778,7 +10797,7 @@
       </c>
       <c r="R181" s="1"/>
     </row>
-    <row r="182" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>181</v>
       </c>
@@ -10830,7 +10849,7 @@
       </c>
       <c r="R182" s="1"/>
     </row>
-    <row r="183" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>182</v>
       </c>
@@ -10882,7 +10901,7 @@
       </c>
       <c r="R183" s="1"/>
     </row>
-    <row r="184" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>183</v>
       </c>
@@ -10934,7 +10953,7 @@
       </c>
       <c r="R184" s="1"/>
     </row>
-    <row r="185" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>184</v>
       </c>
@@ -10986,7 +11005,7 @@
       </c>
       <c r="R185" s="1"/>
     </row>
-    <row r="186" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>185</v>
       </c>
@@ -11038,7 +11057,7 @@
       </c>
       <c r="R186" s="1"/>
     </row>
-    <row r="187" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>186</v>
       </c>
@@ -11090,7 +11109,7 @@
       </c>
       <c r="R187" s="1"/>
     </row>
-    <row r="188" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>187</v>
       </c>
@@ -11142,7 +11161,7 @@
       </c>
       <c r="R188" s="1"/>
     </row>
-    <row r="189" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>188</v>
       </c>
@@ -11194,7 +11213,7 @@
       </c>
       <c r="R189" s="1"/>
     </row>
-    <row r="190" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>189</v>
       </c>
@@ -11246,7 +11265,7 @@
       </c>
       <c r="R190" s="1"/>
     </row>
-    <row r="191" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>190</v>
       </c>
@@ -11298,7 +11317,7 @@
       </c>
       <c r="R191" s="1"/>
     </row>
-    <row r="192" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>191</v>
       </c>
@@ -11350,7 +11369,7 @@
       </c>
       <c r="R192" s="1"/>
     </row>
-    <row r="193" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>192</v>
       </c>
@@ -11402,7 +11421,7 @@
       </c>
       <c r="R193" s="1"/>
     </row>
-    <row r="194" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>193</v>
       </c>
@@ -11454,7 +11473,7 @@
       </c>
       <c r="R194" s="1"/>
     </row>
-    <row r="195" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>194</v>
       </c>
@@ -11506,7 +11525,7 @@
       </c>
       <c r="R195" s="1"/>
     </row>
-    <row r="196" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>195</v>
       </c>
@@ -11558,7 +11577,7 @@
       </c>
       <c r="R196" s="1"/>
     </row>
-    <row r="197" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>196</v>
       </c>
@@ -11610,7 +11629,7 @@
       </c>
       <c r="R197" s="1"/>
     </row>
-    <row r="198" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>197</v>
       </c>
@@ -11662,7 +11681,7 @@
       </c>
       <c r="R198" s="1"/>
     </row>
-    <row r="199" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>198</v>
       </c>
@@ -11714,7 +11733,7 @@
       </c>
       <c r="R199" s="1"/>
     </row>
-    <row r="200" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>199</v>
       </c>
@@ -11766,7 +11785,7 @@
       </c>
       <c r="R200" s="1"/>
     </row>
-    <row r="201" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>200</v>
       </c>
@@ -11818,7 +11837,7 @@
       </c>
       <c r="R201" s="1"/>
     </row>
-    <row r="202" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>201</v>
       </c>
@@ -11870,7 +11889,7 @@
       </c>
       <c r="R202" s="1"/>
     </row>
-    <row r="203" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>202</v>
       </c>
@@ -11922,7 +11941,7 @@
       </c>
       <c r="R203" s="1"/>
     </row>
-    <row r="204" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>203</v>
       </c>
@@ -11974,7 +11993,7 @@
       </c>
       <c r="R204" s="1"/>
     </row>
-    <row r="205" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>204</v>
       </c>
@@ -12026,7 +12045,7 @@
       </c>
       <c r="R205" s="1"/>
     </row>
-    <row r="206" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>205</v>
       </c>
@@ -12078,7 +12097,7 @@
       </c>
       <c r="R206" s="1"/>
     </row>
-    <row r="207" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>206</v>
       </c>
@@ -12130,7 +12149,7 @@
       </c>
       <c r="R207" s="1"/>
     </row>
-    <row r="208" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>207</v>
       </c>
@@ -12182,7 +12201,7 @@
       </c>
       <c r="R208" s="1"/>
     </row>
-    <row r="209" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>208</v>
       </c>
@@ -12234,7 +12253,7 @@
       </c>
       <c r="R209" s="1"/>
     </row>
-    <row r="210" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>209</v>
       </c>
@@ -12286,7 +12305,7 @@
       </c>
       <c r="R210" s="1"/>
     </row>
-    <row r="211" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>210</v>
       </c>
@@ -12338,7 +12357,7 @@
       </c>
       <c r="R211" s="1"/>
     </row>
-    <row r="212" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>211</v>
       </c>
@@ -12390,7 +12409,7 @@
       </c>
       <c r="R212" s="1"/>
     </row>
-    <row r="213" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>212</v>
       </c>
@@ -12442,7 +12461,7 @@
       </c>
       <c r="R213" s="1"/>
     </row>
-    <row r="214" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>213</v>
       </c>
@@ -12494,7 +12513,7 @@
       </c>
       <c r="R214" s="1"/>
     </row>
-    <row r="215" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>214</v>
       </c>
@@ -12546,7 +12565,7 @@
       </c>
       <c r="R215" s="1"/>
     </row>
-    <row r="216" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>215</v>
       </c>
@@ -12598,7 +12617,7 @@
       </c>
       <c r="R216" s="1"/>
     </row>
-    <row r="217" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>216</v>
       </c>
@@ -12650,7 +12669,7 @@
       </c>
       <c r="R217" s="1"/>
     </row>
-    <row r="218" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>217</v>
       </c>
@@ -12702,7 +12721,7 @@
       </c>
       <c r="R218" s="1"/>
     </row>
-    <row r="219" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>218</v>
       </c>
@@ -12754,7 +12773,7 @@
       </c>
       <c r="R219" s="1"/>
     </row>
-    <row r="220" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A220" s="1">
         <v>219</v>
       </c>
@@ -12806,7 +12825,7 @@
       </c>
       <c r="R220" s="1"/>
     </row>
-    <row r="221" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A221" s="1">
         <v>220</v>
       </c>
@@ -12858,7 +12877,7 @@
       </c>
       <c r="R221" s="1"/>
     </row>
-    <row r="222" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A222" s="1">
         <v>221</v>
       </c>
@@ -12910,7 +12929,7 @@
       </c>
       <c r="R222" s="1"/>
     </row>
-    <row r="223" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A223" s="1">
         <v>222</v>
       </c>
@@ -12962,7 +12981,7 @@
       </c>
       <c r="R223" s="1"/>
     </row>
-    <row r="224" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A224" s="1">
         <v>223</v>
       </c>
@@ -13014,7 +13033,7 @@
       </c>
       <c r="R224" s="1"/>
     </row>
-    <row r="225" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>224</v>
       </c>
@@ -13066,7 +13085,7 @@
       </c>
       <c r="R225" s="1"/>
     </row>
-    <row r="226" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A226" s="1">
         <v>225</v>
       </c>
@@ -13118,7 +13137,7 @@
       </c>
       <c r="R226" s="1"/>
     </row>
-    <row r="227" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A227" s="1">
         <v>226</v>
       </c>
@@ -13170,7 +13189,7 @@
       </c>
       <c r="R227" s="1"/>
     </row>
-    <row r="228" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A228" s="1">
         <v>227</v>
       </c>
@@ -13222,7 +13241,7 @@
       </c>
       <c r="R228" s="1"/>
     </row>
-    <row r="229" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A229" s="1">
         <v>228</v>
       </c>
@@ -13274,7 +13293,7 @@
       </c>
       <c r="R229" s="1"/>
     </row>
-    <row r="230" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A230" s="1">
         <v>229</v>
       </c>
@@ -13326,7 +13345,7 @@
       </c>
       <c r="R230" s="1"/>
     </row>
-    <row r="231" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A231" s="1">
         <v>230</v>
       </c>
@@ -13379,33 +13398,33 @@
       <c r="R231" s="1"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1:A156">
-    <cfRule type="containsBlanks" dxfId="5" priority="6">
+  <conditionalFormatting sqref="A1:A156 E5:H5 J5:L5">
+    <cfRule type="containsBlanks" dxfId="6" priority="6">
       <formula>LEN(TRIM(A1))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2:B148">
-    <cfRule type="containsBlanks" dxfId="4" priority="5">
+    <cfRule type="containsBlanks" dxfId="5" priority="5">
       <formula>LEN(TRIM(B2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:D156">
-    <cfRule type="containsBlanks" dxfId="3" priority="4">
+    <cfRule type="containsBlanks" dxfId="4" priority="4">
       <formula>LEN(TRIM(C2))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:O144 N145:O194 N195:N203 O195:O231">
-    <cfRule type="containsBlanks" dxfId="2" priority="3">
+  <conditionalFormatting sqref="E2:O4 N145:O194 N195:N203 O195:O231 E6:O144 M5:O5 I5">
+    <cfRule type="containsBlanks" dxfId="3" priority="3">
       <formula>LEN(TRIM(E2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q231">
-    <cfRule type="containsBlanks" dxfId="1" priority="2">
+    <cfRule type="containsBlanks" dxfId="2" priority="2">
       <formula>LEN(TRIM(Q2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E145:M159">
-    <cfRule type="containsBlanks" dxfId="0" priority="1">
+    <cfRule type="containsBlanks" dxfId="1" priority="1">
       <formula>LEN(TRIM(E145))=0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>